<commit_message>
V 0.1.8/j Item PopUp window: now connected with the windowManager
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/AdvancedItemData.xlsx
+++ b/Assets/StreamingAssets/AdvancedItemData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PartDatas" sheetId="1" r:id="rId1"/>
@@ -2428,7 +2428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -19520,8 +19520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19703,7 +19703,7 @@
         <v>1</v>
       </c>
       <c r="U2">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="V2">
         <v>1</v>

</xml_diff>